<commit_message>
use chinese character 囧 as the default value of blank table cell
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344C6A0A-7988-4137-9942-A87475DF966B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150C71E0-6615-430E-A33F-68AC6B48F717}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2676" yWindow="3948" windowWidth="26232" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1C3986B6-1DD0-4044-ABD9-4BDAE5D1E243}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{1C3986B6-1DD0-4044-ABD9-4BDAE5D1E243}">
       <text>
         <r>
           <rPr>
@@ -163,6 +163,34 @@
 3为防御
 4为金币收益
 5为金币价值</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{F96BD10F-9D3C-41E2-9149-B5D467F120F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+BulletNormal
+BulletMissile
+BulletBasicTrace</t>
         </r>
       </text>
     </comment>
@@ -205,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{C7412016-C203-469A-A028-49BFF0D41358}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{C7412016-C203-469A-A028-49BFF0D41358}">
       <text>
         <r>
           <rPr>
@@ -231,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C5EFFE3B-82A3-4DC3-9134-9332A69564A2}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{C5EFFE3B-82A3-4DC3-9134-9332A69564A2}">
       <text>
         <r>
           <rPr>
@@ -257,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{540B4443-5480-4314-B5F8-93E016D6A4CB}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{540B4443-5480-4314-B5F8-93E016D6A4CB}">
       <text>
         <r>
           <rPr>
@@ -284,6 +312,34 @@
 3为防御
 4为金币收益
 5为金币价值</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{7B10D316-1774-4D3A-84AE-C9F5C887653E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+BulletNormal
+BulletMissile
+BulletBasicTrace</t>
         </r>
       </text>
     </comment>
@@ -326,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{46CDAF05-3EB8-4EF7-B12F-DF91D4A05362}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{46CDAF05-3EB8-4EF7-B12F-DF91D4A05362}">
       <text>
         <r>
           <rPr>
@@ -352,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{E52B8337-FCD9-42D3-A368-AF491E15FFEE}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{E52B8337-FCD9-42D3-A368-AF491E15FFEE}">
       <text>
         <r>
           <rPr>
@@ -378,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{BF0E59D3-2B0A-457B-B572-B03F56F78E25}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{BF0E59D3-2B0A-457B-B572-B03F56F78E25}">
       <text>
         <r>
           <rPr>
@@ -405,6 +461,34 @@
 3为防御
 4为金币收益
 5为金币价值</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C835D520-8FA0-47E8-9094-2BBE538357B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+BulletNormal
+BulletMissile
+BulletBasicTrace</t>
         </r>
       </text>
     </comment>
@@ -529,12 +613,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E08E5B62-A112-411E-B3BC-764B0DCB95FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+BulletNormal
+BulletMissile
+BulletBasicTrace</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
   <si>
     <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -700,10 +812,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CoinMultiply</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>装备编号</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1062,6 +1170,49 @@
   <si>
     <t>[0]为图集名，[1]为精灵名</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BulletPrefabName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BulletName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹使用的预制件名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BulletNormal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BulletBasicTrace</t>
+  </si>
+  <si>
+    <t>BulletMissile</t>
+  </si>
+  <si>
+    <t>BulletMissile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulletLightBlue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulletRed</t>
+  </si>
+  <si>
+    <t>bulletSmallBrown</t>
+  </si>
+  <si>
+    <t>bulletMissile1</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1171,6 +1322,14 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1228,13 +1387,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1288,12 +1448,104 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1832,13 +2084,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -1851,25 +2103,26 @@
     <col min="6" max="6" width="8.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="4"/>
+    <col min="9" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29" style="4" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>102</v>
-      </c>
       <c r="C1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>31</v>
@@ -1884,34 +2137,37 @@
         <v>38</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J1" s="17" t="s">
         <v>47</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1949,19 +2205,22 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1976,18 +2235,19 @@
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="18"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O3" s="18"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>43</v>
-      </c>
       <c r="C4" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>35</v>
@@ -2005,36 +2265,39 @@
         <v>40</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>49</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="N4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -2048,17 +2311,18 @@
       <c r="L5" s="16"/>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O5" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>1001</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="16">
         <v>1</v>
@@ -2082,33 +2346,36 @@
         <v>1</v>
       </c>
       <c r="J6" s="16">
+        <v>99</v>
+      </c>
+      <c r="K6" s="16">
         <v>1</v>
       </c>
-      <c r="K6" s="16">
-        <v>99</v>
-      </c>
       <c r="L6" s="16">
-        <v>1</v>
-      </c>
-      <c r="M6" s="16">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>1011</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="16">
         <v>1</v>
@@ -2132,50 +2399,59 @@
         <v>1</v>
       </c>
       <c r="J7" s="16">
+        <v>99</v>
+      </c>
+      <c r="K7" s="16">
         <v>1</v>
       </c>
-      <c r="K7" s="16">
-        <v>99</v>
-      </c>
       <c r="L7" s="16">
-        <v>1</v>
-      </c>
-      <c r="M7" s="16">
         <v>2</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>92</v>
+      <c r="M7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>109</v>
+        <v>141</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="16" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J2">
-    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
+  <conditionalFormatting sqref="A2:I2 P2">
+    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:P2">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+  <conditionalFormatting sqref="J2:O2">
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="N7" r:id="rId1" xr:uid="{1A678028-1066-4B0D-989C-32DDC872CB8C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8026B52-CF55-48DC-8D86-B26C46E34A0E}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2187,17 +2463,18 @@
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
@@ -2205,7 +2482,7 @@
         <v>30</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>31</v>
@@ -2220,34 +2497,37 @@
         <v>38</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J1" s="17" t="s">
         <v>47</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,19 +2565,22 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2312,18 +2595,19 @@
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="18"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="O3" s="18"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>35</v>
@@ -2341,36 +2625,39 @@
         <v>40</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>49</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="N4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="O4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2384,12 +2671,13 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="O5" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2001</v>
       </c>
@@ -2418,28 +2706,31 @@
         <v>1</v>
       </c>
       <c r="J6" s="5">
+        <v>19</v>
+      </c>
+      <c r="K6" s="5">
         <v>1</v>
       </c>
-      <c r="K6" s="5">
-        <v>19</v>
-      </c>
       <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>2011</v>
       </c>
@@ -2468,28 +2759,31 @@
         <v>1</v>
       </c>
       <c r="J7" s="5">
+        <v>19</v>
+      </c>
+      <c r="K7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" s="5">
-        <v>19</v>
-      </c>
       <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>2021</v>
       </c>
@@ -2518,28 +2812,31 @@
         <v>1</v>
       </c>
       <c r="J8" s="5">
+        <v>19</v>
+      </c>
+      <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
-        <v>19</v>
-      </c>
       <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
         <v>8</v>
       </c>
+      <c r="M8" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="N8" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>2031</v>
       </c>
@@ -2568,28 +2865,31 @@
         <v>1</v>
       </c>
       <c r="J9" s="5">
+        <v>19</v>
+      </c>
+      <c r="K9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="5">
-        <v>19</v>
-      </c>
       <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
         <v>12</v>
       </c>
+      <c r="M9" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="N9" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>2041</v>
       </c>
@@ -2618,43 +2918,52 @@
         <v>1</v>
       </c>
       <c r="J10" s="5">
+        <v>19</v>
+      </c>
+      <c r="K10" s="5">
         <v>1</v>
       </c>
-      <c r="K10" s="5">
-        <v>19</v>
-      </c>
       <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
         <v>24</v>
       </c>
+      <c r="M10" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="N10" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>109</v>
+        <v>98</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:P2">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:O2">
+    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2664,10 +2973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CF833-C8E3-4FD3-833A-20A74CDB8951}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2679,25 +2988,26 @@
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>102</v>
-      </c>
       <c r="C1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>31</v>
@@ -2712,34 +3022,37 @@
         <v>38</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J1" s="17" t="s">
         <v>47</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2777,19 +3090,22 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2804,18 +3120,19 @@
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="18"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="O3" s="18"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>35</v>
@@ -2833,36 +3150,39 @@
         <v>40</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>49</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="N4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="O4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2874,19 +3194,20 @@
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="O5" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3001</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="14">
         <v>3</v>
@@ -2910,33 +3231,36 @@
         <v>1</v>
       </c>
       <c r="J6" s="5">
+        <v>49</v>
+      </c>
+      <c r="K6" s="5">
         <v>1</v>
       </c>
-      <c r="K6" s="5">
-        <v>49</v>
-      </c>
       <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3011</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="14">
         <v>3</v>
@@ -2960,28 +3284,31 @@
         <v>1</v>
       </c>
       <c r="J7" s="5">
+        <v>49</v>
+      </c>
+      <c r="K7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" s="5">
-        <v>49</v>
-      </c>
       <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>3021</v>
       </c>
@@ -3010,28 +3337,31 @@
         <v>1</v>
       </c>
       <c r="J8" s="5">
+        <v>49</v>
+      </c>
+      <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
-        <v>49</v>
-      </c>
       <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
         <v>21</v>
       </c>
+      <c r="M8" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="N8" s="16" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3031</v>
       </c>
@@ -3060,28 +3390,31 @@
         <v>1</v>
       </c>
       <c r="J9" s="5">
+        <v>49</v>
+      </c>
+      <c r="K9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="5">
-        <v>49</v>
-      </c>
       <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
         <v>22</v>
       </c>
+      <c r="M9" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="N9" s="16" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>3041</v>
       </c>
@@ -3110,37 +3443,46 @@
         <v>1</v>
       </c>
       <c r="J10" s="5">
+        <v>49</v>
+      </c>
+      <c r="K10" s="5">
         <v>1</v>
       </c>
-      <c r="K10" s="5">
-        <v>49</v>
-      </c>
       <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
         <v>32</v>
       </c>
+      <c r="M10" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="N10" s="16" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:M2">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  <conditionalFormatting sqref="M2:O2">
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:P2">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  <conditionalFormatting sqref="P2">
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:L2">
+    <cfRule type="duplicateValues" dxfId="8" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3149,10 +3491,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1034E8-97B7-4AE6-85D3-98B9692FAA0B}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3171,17 +3513,19 @@
     <col min="14" max="14" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>31</v>
@@ -3196,34 +3540,40 @@
         <v>38</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N1" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="P1" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3264,16 +3614,22 @@
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3290,16 +3646,18 @@
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
       <c r="P3" s="18"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>35</v>
@@ -3317,36 +3675,42 @@
         <v>40</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="L4" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="P4" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3362,15 +3726,17 @@
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
       <c r="P5" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4001</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="14">
         <v>4</v>
@@ -3403,24 +3769,26 @@
         <v>1</v>
       </c>
       <c r="M6" s="5">
-        <v>2222</v>
+        <v>5</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4011</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="14">
         <v>4</v>
@@ -3453,33 +3821,41 @@
         <v>1</v>
       </c>
       <c r="M7" s="5">
-        <v>3333</v>
+        <v>122</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>112</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A5">
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:M2">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  <conditionalFormatting sqref="N2:P2">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:M2">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:P2">
+  <conditionalFormatting sqref="R2">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3517,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -3542,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,7 +3926,7 @@
         <v>100</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3558,7 +3934,7 @@
         <v>101</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3566,7 +3942,7 @@
         <v>102</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,7 +3950,7 @@
         <v>103</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3582,7 +3958,7 @@
         <v>104</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3590,7 +3966,7 @@
         <v>105</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3598,7 +3974,7 @@
         <v>1010</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3606,7 +3982,7 @@
         <v>1011</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3614,7 +3990,7 @@
         <v>1012</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3622,7 +3998,7 @@
         <v>1013</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3630,7 +4006,7 @@
         <v>1014</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3638,7 +4014,7 @@
         <v>1020</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3646,7 +4022,7 @@
         <v>1021</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3654,7 +4030,7 @@
         <v>1022</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3662,7 +4038,7 @@
         <v>1023</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3670,7 +4046,7 @@
         <v>1024</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3678,7 +4054,7 @@
         <v>1030</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3686,7 +4062,7 @@
         <v>1031</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3694,7 +4070,7 @@
         <v>2000</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3702,7 +4078,7 @@
         <v>2001</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3710,7 +4086,7 @@
         <v>2002</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3718,7 +4094,7 @@
         <v>2003</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3726,7 +4102,7 @@
         <v>2004</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3887,24 +4263,24 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>9999</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3952,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
@@ -3972,10 +4348,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
         <v>131</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -3984,10 +4360,10 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="9"/>
     </row>
@@ -3996,7 +4372,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -4008,7 +4384,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -4016,10 +4392,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -4027,10 +4403,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
modify vector3 to Vector3
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CF3E33-6EB2-4D3F-8D32-2C11B7A406BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8002E5-640D-4B66-9FB5-5086166AD6CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="564" windowWidth="32796" windowHeight="15576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{540B4443-5480-4314-B5F8-93E016D6A4CB}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{540B4443-5480-4314-B5F8-93E016D6A4CB}">
       <text>
         <r>
           <rPr>
@@ -281,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{7B10D316-1774-4D3A-84AE-C9F5C887653E}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{7B10D316-1774-4D3A-84AE-C9F5C887653E}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{BF0E59D3-2B0A-457B-B572-B03F56F78E25}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{BF0E59D3-2B0A-457B-B572-B03F56F78E25}">
       <text>
         <r>
           <rPr>
@@ -401,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C835D520-8FA0-47E8-9094-2BBE538357B3}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{C835D520-8FA0-47E8-9094-2BBE538357B3}">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C4B0E261-EB9F-43EB-A6F8-4FB7B1B7F5D0}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{C4B0E261-EB9F-43EB-A6F8-4FB7B1B7F5D0}">
       <text>
         <r>
           <rPr>
@@ -521,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E08E5B62-A112-411E-B3BC-764B0DCB95FA}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{E08E5B62-A112-411E-B3BC-764B0DCB95FA}">
       <text>
         <r>
           <rPr>
@@ -554,7 +554,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="170">
   <si>
     <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1092,10 +1092,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>预制件名称</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1104,16 +1100,132 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>vector3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>预制件的坐标</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0|0.19|0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>0|0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>body10001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>body20001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun11001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun21001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile12001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun21011</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun21021</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun21031</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile22001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile22011</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile22021</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile22031</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missile22041</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|-0.18|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.15|-0.5|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.17|-0.5|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.22|-0.31|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.31|-0.4|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙虾钳子</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlaneFactory</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gun21041</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.21|-0.37|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.31|0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.31|0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.43|-0.23|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.37|-0.29|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.59|0.03|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vector3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1238,7 +1350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1279,6 +1391,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1286,7 +1409,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1344,12 +1467,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1975,10 +2170,10 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -2050,7 +2245,7 @@
         <v>135</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>97</v>
@@ -2106,10 +2301,10 @@
         <v>91</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
@@ -2186,10 +2381,10 @@
         <v>78</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q4" s="18" t="s">
         <v>94</v>
@@ -2270,8 +2465,12 @@
       <c r="N6" s="16">
         <v>10001</v>
       </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
+      <c r="O6" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="Q6" s="16" t="s">
         <v>95</v>
       </c>
@@ -2325,9 +2524,11 @@
       <c r="N7" s="16">
         <v>20001</v>
       </c>
-      <c r="O7" s="16"/>
+      <c r="O7" s="16" t="s">
+        <v>141</v>
+      </c>
       <c r="P7" s="16" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="Q7" s="16" t="s">
         <v>95</v>
@@ -2342,16 +2543,19 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="23" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2 A2:I2">
-    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
+  <conditionalFormatting sqref="A2:I2">
+    <cfRule type="duplicateValues" dxfId="26" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:L2">
+    <cfRule type="duplicateValues" dxfId="25" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:Q2">
-    <cfRule type="duplicateValues" dxfId="20" priority="32"/>
+  <conditionalFormatting sqref="M2:R2">
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2361,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8026B52-CF55-48DC-8D86-B26C46E34A0E}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2382,12 +2586,13 @@
     <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
@@ -2431,16 +2636,22 @@
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2487,13 +2698,19 @@
         <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="R2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2508,11 +2725,13 @@
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="18"/>
+      <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -2555,17 +2774,23 @@
       <c r="N4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>55</v>
       </c>
@@ -2584,13 +2809,15 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>11001</v>
       </c>
@@ -2634,16 +2861,22 @@
         <v>11001</v>
       </c>
       <c r="O6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="R6" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="S6" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>21001</v>
       </c>
@@ -2687,16 +2920,22 @@
         <v>21001</v>
       </c>
       <c r="O7" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="R7" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="S7" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>21011</v>
       </c>
@@ -2740,16 +2979,22 @@
         <v>21011</v>
       </c>
       <c r="O8" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="R8" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="Q8" s="16" t="s">
+      <c r="S8" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>21021</v>
       </c>
@@ -2793,16 +3038,22 @@
         <v>21021</v>
       </c>
       <c r="O9" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q9" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="R9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="S9" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>21031</v>
       </c>
@@ -2846,37 +3097,108 @@
         <v>21031</v>
       </c>
       <c r="O10" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="R10" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="S10" s="19" t="s">
         <v>124</v>
       </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>21041</v>
+      </c>
+      <c r="B11" s="24">
+        <v>1015</v>
+      </c>
+      <c r="C11" s="24">
+        <v>2</v>
+      </c>
+      <c r="D11" s="24">
+        <v>3</v>
+      </c>
+      <c r="E11" s="24">
+        <v>3</v>
+      </c>
+      <c r="F11" s="25">
+        <v>0</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0</v>
+      </c>
+      <c r="I11" s="26">
+        <v>1</v>
+      </c>
+      <c r="J11" s="26">
+        <v>33</v>
+      </c>
+      <c r="K11" s="26">
+        <v>1</v>
+      </c>
+      <c r="L11" s="26">
+        <v>25</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="N11" s="24">
+        <v>21041</v>
+      </c>
+      <c r="O11" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q11" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K13" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
-    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O2">
-    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:N2 Q2">
+    <cfRule type="duplicateValues" dxfId="18" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2">
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2">
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:P2">
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2886,10 +3208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CF833-C8E3-4FD3-833A-20A74CDB8951}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2907,12 +3229,13 @@
     <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>92</v>
       </c>
@@ -2956,16 +3279,22 @@
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3012,13 +3341,19 @@
         <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="R2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3033,11 +3368,13 @@
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="18"/>
+      <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -3080,17 +3417,23 @@
       <c r="N4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>55</v>
       </c>
@@ -3109,13 +3452,15 @@
       <c r="L5" s="14"/>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>12001</v>
       </c>
@@ -3159,16 +3504,22 @@
         <v>12001</v>
       </c>
       <c r="O6" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="R6" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="S6" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>22001</v>
       </c>
@@ -3212,16 +3563,22 @@
         <v>22001</v>
       </c>
       <c r="O7" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="R7" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="S7" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>22011</v>
       </c>
@@ -3265,16 +3622,22 @@
         <v>22011</v>
       </c>
       <c r="O8" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="R8" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="S8" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>22021</v>
       </c>
@@ -3318,16 +3681,22 @@
         <v>22021</v>
       </c>
       <c r="O9" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q9" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="R9" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="Q9" s="20" t="s">
+      <c r="S9" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>22031</v>
       </c>
@@ -3371,16 +3740,22 @@
         <v>22031</v>
       </c>
       <c r="O10" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="R10" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="S10" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>22041</v>
       </c>
@@ -3424,84 +3799,40 @@
         <v>22041</v>
       </c>
       <c r="O11" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q11" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P11" s="19" t="s">
+      <c r="R11" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="Q11" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>22051</v>
-      </c>
-      <c r="B12" s="16">
-        <v>1026</v>
-      </c>
-      <c r="C12" s="14">
-        <v>3</v>
-      </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
-        <v>12</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>49</v>
-      </c>
-      <c r="K12" s="5">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5">
-        <v>32</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N12" s="16">
-        <v>22051</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q12" s="20" t="s">
+      <c r="S11" s="20" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O2">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+  <conditionalFormatting sqref="M2:N2 Q2">
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  <conditionalFormatting sqref="R2">
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  <conditionalFormatting sqref="S2">
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L2">
-    <cfRule type="duplicateValues" dxfId="8" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:P2">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3510,9 +3841,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1034E8-97B7-4AE6-85D3-98B9692FAA0B}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3529,12 +3862,13 @@
     <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -3581,16 +3915,22 @@
         <v>76</v>
       </c>
       <c r="P1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3640,13 +3980,19 @@
         <v>91</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="S2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3662,11 +4008,13 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
-      <c r="P3" s="18"/>
+      <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="R3" s="18"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+    </row>
+    <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -3712,17 +4060,23 @@
       <c r="O4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="R4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="T4" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>55</v>
       </c>
@@ -3742,13 +4096,15 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+    </row>
+    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4001</v>
       </c>
@@ -3794,13 +4150,17 @@
       <c r="O6" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="R6" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+    </row>
+    <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4011</v>
       </c>
@@ -3846,33 +4206,40 @@
       <c r="O7" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="R7" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:M2">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:P2">
+  <conditionalFormatting sqref="N2:O2 R2">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2">
+  <conditionalFormatting sqref="T2">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2">
+  <conditionalFormatting sqref="P2:Q2">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3882,10 +4249,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4028,113 +4395,121 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
-        <v>1020</v>
+        <v>1015</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
-        <v>2000</v>
+        <v>1031</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
+        <v>2003</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
         <v>2004</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B32" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4331,7 +4706,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
begin to refactor this project
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8002E5-640D-4B66-9FB5-5086166AD6CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221D1861-F435-4C0D-9E63-6675191EE204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -1350,7 +1350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1391,17 +1391,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1409,7 +1398,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1467,28 +1456,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2169,7 +2155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -2565,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8026B52-CF55-48DC-8D86-B26C46E34A0E}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2810,7 +2796,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="4"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="18" t="s">
         <v>96</v>
       </c>
@@ -2981,7 +2967,7 @@
       <c r="O8" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="22" t="s">
         <v>155</v>
       </c>
       <c r="Q8" s="16" t="s">
@@ -3040,7 +3026,7 @@
       <c r="O9" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="21" t="s">
         <v>156</v>
       </c>
       <c r="Q9" s="16" t="s">
@@ -3099,7 +3085,7 @@
       <c r="O10" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="22" t="s">
+      <c r="P10" s="21" t="s">
         <v>157</v>
       </c>
       <c r="Q10" s="16" t="s">
@@ -3113,55 +3099,55 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="23">
         <v>21041</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>1015</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>3</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="23">
         <v>3</v>
       </c>
-      <c r="F11" s="25">
-        <v>0</v>
-      </c>
-      <c r="G11" s="25">
-        <v>0</v>
-      </c>
-      <c r="H11" s="25">
-        <v>0</v>
-      </c>
-      <c r="I11" s="26">
+      <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25">
         <v>1</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <v>33</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <v>1</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="25">
         <v>25</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="23">
         <v>21041</v>
       </c>
-      <c r="O11" s="27" t="s">
+      <c r="O11" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="P11" s="28" t="s">
+      <c r="P11" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="Q11" s="27" t="s">
+      <c r="Q11" s="26" t="s">
         <v>163</v>
       </c>
       <c r="R11" s="19" t="s">
@@ -3170,9 +3156,6 @@
       <c r="S11" s="19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K13" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3506,7 +3489,7 @@
       <c r="O6" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" s="21" t="s">
         <v>164</v>
       </c>
       <c r="Q6" s="16" t="s">
@@ -3565,7 +3548,7 @@
       <c r="O7" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="21" t="s">
         <v>165</v>
       </c>
       <c r="Q7" s="16" t="s">
@@ -3624,7 +3607,7 @@
       <c r="O8" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="21" t="s">
         <v>158</v>
       </c>
       <c r="Q8" s="16" t="s">
@@ -3683,7 +3666,7 @@
       <c r="O9" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="21" t="s">
         <v>166</v>
       </c>
       <c r="Q9" s="16" t="s">
@@ -3742,7 +3725,7 @@
       <c r="O10" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="P10" s="22" t="s">
+      <c r="P10" s="21" t="s">
         <v>167</v>
       </c>
       <c r="Q10" s="16" t="s">
@@ -3801,7 +3784,7 @@
       <c r="O11" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="21" t="s">
         <v>168</v>
       </c>
       <c r="Q11" s="16" t="s">

</xml_diff>

<commit_message>
refactor over,but output lua setting is not finished
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221D1861-F435-4C0D-9E63-6675191EE204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA6EDFF-A916-49B4-A776-0A12F69961D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="LanguageSetting" sheetId="3" r:id="rId5"/>
     <sheet name="GameSetting" sheetId="2" r:id="rId6"/>
     <sheet name="IconSetting" sheetId="9" r:id="rId7"/>
+    <sheet name="GermSetting" sheetId="10" r:id="rId8"/>
+    <sheet name="说明" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -553,8 +555,45 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{FB01834C-4712-4D78-9FCE-8ECFCA6B9C0B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1：为血量暴多细菌
+2：为分裂细菌
+100及之后为非细菌生成器产生的细菌
+100：为分裂细菌分裂后产生的细菌</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="192">
   <si>
     <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1046,20 +1085,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>BulletNormal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BulletBasicTrace</t>
-  </si>
-  <si>
-    <t>BulletMissile</t>
-  </si>
-  <si>
-    <t>BulletMissile</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>bulletLightBlue</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1226,6 +1251,108 @@
   <si>
     <t>Vector3</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量值不足{0}点，无法开始游戏</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有解锁的尾翼部件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有解锁的导弹部件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有解锁的副武器部件</t>
+  </si>
+  <si>
+    <t>没有解锁的机身部件</t>
+  </si>
+  <si>
+    <t>未解锁，请通关关卡{0}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>细菌名字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟具体细菌的类名字一致</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预制体名字</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>guaiwu1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>guaiwu2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radius</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>细菌半径</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>细菌id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID唯一标识细菌类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动速度</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletNormal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletNormal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletBasicTrace</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletDirectionTrace</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletMissile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletMissile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.GermBoom</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.GermBounce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGame.Logic.BulletNormal2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1235,7 +1362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1335,6 +1462,19 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1350,7 +1490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1391,6 +1531,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1398,7 +1562,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1477,12 +1641,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2153,13 +2380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -2179,8 +2406,8 @@
     <col min="14" max="14" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="19.88671875" style="4" customWidth="1"/>
     <col min="17" max="17" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" style="4" customWidth="1"/>
-    <col min="19" max="19" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -2228,10 +2455,10 @@
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>97</v>
@@ -2290,7 +2517,7 @@
         <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
@@ -2302,186 +2529,148 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+    <row r="3" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="O4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>122</v>
-      </c>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="Q5" s="18" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="Q6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
-        <v>10001</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="E6" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="16">
-        <v>0</v>
-      </c>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16">
-        <v>0</v>
-      </c>
-      <c r="I6" s="16">
-        <v>1</v>
-      </c>
-      <c r="J6" s="16">
-        <v>99</v>
-      </c>
-      <c r="K6" s="16">
-        <v>1</v>
-      </c>
-      <c r="L6" s="16">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="N6" s="16">
-        <v>10001</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
-        <v>20001</v>
+        <v>10001</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="16">
         <v>1</v>
       </c>
       <c r="D7" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="16">
         <v>0</v>
@@ -2502,46 +2691,105 @@
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N7" s="16">
-        <v>20001</v>
+        <v>10001</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="Q7" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R7" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="16">
+        <v>20001</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="16">
+        <v>1</v>
+      </c>
+      <c r="J8" s="16">
+        <v>99</v>
+      </c>
+      <c r="K8" s="16">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <v>2</v>
+      </c>
+      <c r="M8" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="16" t="s">
-        <v>123</v>
+      <c r="N8" s="16">
+        <v>20001</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="27" priority="31"/>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="duplicateValues" dxfId="31" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" dxfId="26" priority="11"/>
+  <conditionalFormatting sqref="A2:I3">
+    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:L2">
-    <cfRule type="duplicateValues" dxfId="25" priority="37"/>
+  <conditionalFormatting sqref="J2:L3">
+    <cfRule type="duplicateValues" dxfId="29" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2">
-    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
+  <conditionalFormatting sqref="S2:S3">
+    <cfRule type="duplicateValues" dxfId="28" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:R2">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+  <conditionalFormatting sqref="M2:R3">
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2551,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8026B52-CF55-48DC-8D86-B26C46E34A0E}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2575,7 +2823,7 @@
     <col min="15" max="16" width="14.33203125" customWidth="1"/>
     <col min="17" max="17" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2622,10 +2870,10 @@
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>97</v>
@@ -2684,7 +2932,7 @@
         <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
@@ -2696,187 +2944,149 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="18" t="s">
+      <c r="O5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q5" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R5" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="S5" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>11001</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1010</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>33</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
-        <v>3</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="N6" s="14">
-        <v>11001</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>21001</v>
+        <v>11001</v>
       </c>
       <c r="B7" s="8">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7" s="5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="12">
         <v>0</v>
@@ -2897,45 +3107,45 @@
         <v>1</v>
       </c>
       <c r="L7" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N7" s="14">
-        <v>21001</v>
+        <v>11001</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="Q7" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>21011</v>
-      </c>
-      <c r="B8" s="14">
-        <v>1012</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="A8" s="5">
+        <v>21001</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1011</v>
+      </c>
+      <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="14">
-        <v>1.3</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1.3</v>
+      <c r="D8" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1.2</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
@@ -2956,45 +3166,45 @@
         <v>1</v>
       </c>
       <c r="L8" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N8" s="14">
-        <v>21011</v>
+        <v>21001</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>155</v>
+        <v>139</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="Q8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="R8" s="19" t="s">
-        <v>129</v>
+      <c r="R8" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>21021</v>
+        <v>21011</v>
       </c>
       <c r="B9" s="14">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C9" s="14">
         <v>2</v>
       </c>
       <c r="D9" s="14">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E9" s="14">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="F9" s="12">
         <v>0</v>
@@ -3015,45 +3225,45 @@
         <v>1</v>
       </c>
       <c r="L9" s="5">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N9" s="14">
-        <v>21021</v>
+        <v>21011</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>151</v>
       </c>
       <c r="Q9" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>21031</v>
+        <v>21021</v>
       </c>
       <c r="B10" s="14">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C10" s="14">
         <v>2</v>
       </c>
       <c r="D10" s="14">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="14">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F10" s="12">
         <v>0</v>
@@ -3074,114 +3284,173 @@
         <v>1</v>
       </c>
       <c r="L10" s="5">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N10" s="14">
-        <v>21031</v>
+        <v>21021</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="Q10" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="14">
+        <v>21031</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1014</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>33</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5">
+        <v>24</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="N11" s="14">
+        <v>21031</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
         <v>21041</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B12" s="23">
         <v>1015</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C12" s="23">
         <v>2</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D12" s="23">
         <v>3</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E12" s="23">
         <v>3</v>
       </c>
-      <c r="F11" s="24">
-        <v>0</v>
-      </c>
-      <c r="G11" s="24">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="25">
+      <c r="F12" s="24">
+        <v>0</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
+      <c r="I12" s="25">
         <v>1</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J12" s="25">
         <v>33</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K12" s="25">
         <v>1</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L12" s="25">
         <v>25</v>
       </c>
-      <c r="M11" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="N11" s="23">
+      <c r="M12" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="N12" s="23">
         <v>21041</v>
       </c>
-      <c r="O11" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q11" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="R11" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>124</v>
+      <c r="O12" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="P12" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q12" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="22" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
+  <conditionalFormatting sqref="A2:A6">
+    <cfRule type="duplicateValues" dxfId="24" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2">
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
+  <conditionalFormatting sqref="Q2:Q3">
+    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:N2 Q2">
-    <cfRule type="duplicateValues" dxfId="18" priority="30"/>
+  <conditionalFormatting sqref="A2:N3 Q2:Q3">
+    <cfRule type="duplicateValues" dxfId="22" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2">
-    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+  <conditionalFormatting sqref="R2:R3">
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+  <conditionalFormatting sqref="S2:S3">
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:P2">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+  <conditionalFormatting sqref="O2:P3">
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3191,10 +3460,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CF833-C8E3-4FD3-833A-20A74CDB8951}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3215,7 +3484,7 @@
     <col min="15" max="16" width="14.33203125" customWidth="1"/>
     <col min="17" max="17" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3262,10 +3531,10 @@
         <v>76</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>97</v>
@@ -3324,7 +3593,7 @@
         <v>91</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>91</v>
@@ -3336,187 +3605,149 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" s="18" t="s">
+      <c r="O5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q5" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="R5" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="S5" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="18" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>12001</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="14">
-        <v>3</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
-        <v>4</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>49</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
-        <v>4</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N6" s="16">
-        <v>12001</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>126</v>
-      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>22001</v>
+        <v>12001</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="14">
         <v>3</v>
       </c>
       <c r="D7" s="12">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E7" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="12">
         <v>0</v>
@@ -3537,45 +3768,45 @@
         <v>1</v>
       </c>
       <c r="L7" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N7" s="16">
-        <v>22001</v>
+        <v>12001</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="Q7" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>22011</v>
-      </c>
-      <c r="B8" s="16">
-        <v>1022</v>
-      </c>
-      <c r="C8" s="16">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>22001</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="14">
         <v>3</v>
       </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16">
-        <v>7</v>
+      <c r="D8" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
@@ -3596,45 +3827,45 @@
         <v>1</v>
       </c>
       <c r="L8" s="5">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N8" s="16">
-        <v>22011</v>
+        <v>22001</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="Q8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="R8" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="S8" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="R8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>22021</v>
+        <v>22011</v>
       </c>
       <c r="B9" s="16">
-        <v>1023</v>
-      </c>
-      <c r="C9" s="14">
+        <v>1022</v>
+      </c>
+      <c r="C9" s="16">
         <v>3</v>
       </c>
       <c r="D9" s="16">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9" s="12">
         <v>0</v>
@@ -3655,45 +3886,45 @@
         <v>1</v>
       </c>
       <c r="L9" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N9" s="16">
-        <v>22021</v>
+        <v>22011</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="Q9" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>22031</v>
+        <v>22021</v>
       </c>
       <c r="B10" s="16">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C10" s="14">
         <v>3</v>
       </c>
       <c r="D10" s="16">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E10" s="16">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10" s="12">
         <v>0</v>
@@ -3714,36 +3945,36 @@
         <v>1</v>
       </c>
       <c r="L10" s="5">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N10" s="16">
-        <v>22031</v>
+        <v>22021</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="Q10" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
-        <v>22041</v>
+        <v>22031</v>
       </c>
       <c r="B11" s="16">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C11" s="14">
         <v>3</v>
@@ -3776,46 +4007,105 @@
         <v>32</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="N11" s="16">
-        <v>22041</v>
+        <v>22031</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="Q11" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="S11" s="20" t="s">
-        <v>125</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>22041</v>
+      </c>
+      <c r="B12" s="16">
+        <v>1025</v>
+      </c>
+      <c r="C12" s="14">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>12</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>49</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>32</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="N12" s="16">
+        <v>22041</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="S12" s="20" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N2 Q2">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+  <conditionalFormatting sqref="M2:N3 Q2:Q3">
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+  <conditionalFormatting sqref="R2:R3">
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+  <conditionalFormatting sqref="S2:S3">
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:L2">
-    <cfRule type="duplicateValues" dxfId="10" priority="31"/>
+  <conditionalFormatting sqref="A2:L3">
+    <cfRule type="duplicateValues" dxfId="14" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:P2">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  <conditionalFormatting sqref="O2:P3">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3824,10 +4114,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1034E8-97B7-4AE6-85D3-98B9692FAA0B}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3898,10 +4188,10 @@
         <v>76</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R1" s="17" t="s">
         <v>97</v>
@@ -3963,7 +4253,7 @@
         <v>91</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>91</v>
@@ -3975,180 +4265,146 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+    </row>
+    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="R4" s="18" t="s">
+      <c r="P5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="S5" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="T4" s="16" t="s">
+      <c r="T5" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="18" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>4001</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="14">
-        <v>4</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="5">
-        <v>199</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5">
-        <v>5</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
     </row>
     <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>4011</v>
+        <v>4001</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="14">
         <v>4</v>
@@ -4181,49 +4437,105 @@
         <v>1</v>
       </c>
       <c r="M7" s="5">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
+    </row>
+    <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>4011</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="14">
+        <v>4</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5">
+        <v>199</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>122</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:M2">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="A2:M3">
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:O2 R2">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="N2:O3 R2:R3">
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  <conditionalFormatting sqref="S2:S3">
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="T2:T3">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:Q2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="P2:Q3">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4232,10 +4544,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4265,241 +4577,294 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>1</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>102</v>
-      </c>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
-        <v>1010</v>
+        <v>105</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
-        <v>1020</v>
+        <v>1015</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
-        <v>2000</v>
+        <v>1031</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
+        <v>2003</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
         <v>2004</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>3000</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>3001</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>3002</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>3003</v>
+      </c>
+      <c r="B37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>3004</v>
+      </c>
+      <c r="B38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>3005</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:C2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A2:C3">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4508,10 +4873,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4548,129 +4913,132 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>4000</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>800</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>9999</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>9999</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>9999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4686,10 +5054,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16613BD9-1BB8-4B3A-9C31-59A58E5C044A}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4726,80 +5094,83 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" t="s">
-        <v>118</v>
-      </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>111</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>116</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4811,4 +5182,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232EF6F-E003-41C5-BAF0-3BEF584E0537}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.74</v>
+      </c>
+      <c r="E8" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>100</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.74</v>
+      </c>
+      <c r="E9" s="19">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B4:B6 B9">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E3">
+    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F377421E-B907-459B-97D2-7B00629910A7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add support for int[] and float[],but you should use an extention method to convert from string[].also add a Test table used for test.
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2655B668-B88E-4268-94B4-83CB560CD95E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A73D5B9-049D-4DC8-B5BF-4C6833D672A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,8 @@
     <sheet name="GameSetting" sheetId="2" r:id="rId6"/>
     <sheet name="IconSetting" sheetId="9" r:id="rId7"/>
     <sheet name="GermSetting" sheetId="10" r:id="rId8"/>
-    <sheet name="说明" sheetId="11" r:id="rId9"/>
+    <sheet name="Test" sheetId="12" r:id="rId9"/>
+    <sheet name="说明Describle" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -593,7 +594,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="217">
   <si>
     <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1359,10 +1360,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>nil</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -1371,6 +1368,89 @@
   </si>
   <si>
     <t>null</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SupportType:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Field annotation:</t>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>float[]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vector3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>xx3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>xx4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>float[]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1495,7 +1575,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1506,6 +1586,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1581,7 +1673,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1675,12 +1767,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2586,25 +2764,25 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>135</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -2834,23 +3012,92 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="duplicateValues" dxfId="31" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I3">
-    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L3">
-    <cfRule type="duplicateValues" dxfId="29" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="duplicateValues" dxfId="28" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:R2 M3:O3 Q3:R3">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F377421E-B907-459B-97D2-7B00629910A7}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3039,25 +3286,25 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>135</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
@@ -3524,28 +3771,28 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="26" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="25" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="24" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q3">
-    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:N3 Q2:Q3">
-    <cfRule type="duplicateValues" dxfId="22" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R3">
-    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:P2 O3">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3738,25 +3985,25 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>192</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
@@ -4223,22 +4470,22 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:N3 Q2:Q3">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R3">
-    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:L3">
-    <cfRule type="duplicateValues" dxfId="14" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:P3">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4250,7 +4497,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4439,25 +4686,25 @@
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="Q3" s="16" t="s">
         <v>135</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
@@ -4687,28 +4934,28 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:M3">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O3 R2:R3">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T3">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:Q2 P3">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4754,7 +5001,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="32"/>
     </row>
@@ -5041,7 +5288,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A2:C3">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5091,7 +5338,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5278,10 +5525,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -5377,8 +5624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232EF6F-E003-41C5-BAF0-3BEF584E0537}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5428,10 +5675,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -5529,16 +5776,16 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B4:B6 B9">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E3">
-    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="39"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5547,15 +5794,188 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F377421E-B907-459B-97D2-7B00629910A7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CFF3D8-2A70-4590-A4A3-4A4431F09686}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>100</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B4:B6 B9">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E3">
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add README.md,other small rectify
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据_程序用.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24270DD-55CC-4ABF-AA33-5D5DC11BD1DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BDDFD-5B96-4C02-88FB-22C8E54DC11E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="1920" windowWidth="21348" windowHeight="12708" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="948" windowWidth="24840" windowHeight="12708" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BodySetting" sheetId="1" r:id="rId1"/>
@@ -2272,7 +2272,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -2712,7 +2712,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3633,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18CF833-C8E3-4FD3-833A-20A74CDB8951}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4308,7 +4308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1034E8-97B7-4AE6-85D3-98B9692FAA0B}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -5094,7 +5094,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5579,7 +5579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B249AD-CC02-4CA9-8D85-7492A456795D}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>